<commit_message>
Atualização de importação de amabas operações e ajustes na planilha.
</commit_message>
<xml_diff>
--- a/Exemplo de arquivo texto/plano_contas.xlsx
+++ b/Exemplo de arquivo texto/plano_contas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evald\OneDrive\Pessoal\Concept\Projeto Contabilidade\Arquivos de teste\Fontes das Macros\Exemplo de arquivo texto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="202C6F0DC72E01CED467D95D4C0D48E77BF41E41" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{FA923932-A5A9-4FD8-A30C-D43AA52E1823}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="202C6F0DC72E01CED467D95D4C0D48E77BF41E41" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{F94EBBCF-B633-4210-A588-925F51418E76}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>